<commit_message>
Updated templates which are used to test template-related services
</commit_message>
<xml_diff>
--- a/catalogue-service-micro/src/test/resources/template/product_data_template.xlsx
+++ b/catalogue-service-micro/src/test/resources/template/product_data_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Information" sheetId="1" state="visible" r:id="rId2"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="236">
   <si>
     <t xml:space="preserve">How to fill in this template?</t>
   </si>
@@ -125,7 +125,7 @@
     <t xml:space="preserve">        NUMBER : The data type that should be specified for properties representing numeric values</t>
   </si>
   <si>
-    <t xml:space="preserve">        QUANTITY : If a numeric property must have an associated unit (e.g. a dimension property), such a property must have QUANTITY type.</t>
+    <t xml:space="preserve">        QUANTITY : If a numeric property must have an associated unit (e.g. a dimension property), such a property must have QUANTITY type. Each quantity property is represented by two adjacent columns QUANTITY VALUE and QUANTITY UNIT.</t>
   </si>
   <si>
     <t xml:space="preserve">        FILE : When a file (image, pdf, etc.) is to be specified for a property (e.g. images, safety sheet, etc.), this data type is used. You should specify the location of the file on your system e.g. C:\Documents\safetysheet.pdf.</t>
@@ -323,252 +323,282 @@
     <t xml:space="preserve">MULTILINGUAL TEXT</t>
   </si>
   <si>
+    <t xml:space="preserve">QUANTITY VALUE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QUANTITY UNIT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NUMBER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BOOLEAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Property Unit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Product_id1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plastic-head mallet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mallet that can be used mosaic tiling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">83</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">43</t>
+  </si>
+  <si>
+    <t xml:space="preserve">315</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RED|GREEN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Product_id2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Iron-head mallet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Strong mallet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">78</t>
+  </si>
+  <si>
+    <t xml:space="preserve">35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">300</t>
+  </si>
+  <si>
+    <t xml:space="preserve">industry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Product_id3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wood-head mallet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Great for metal working</t>
+  </si>
+  <si>
+    <t xml:space="preserve">80</t>
+  </si>
+  <si>
+    <t xml:space="preserve">40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">320</t>
+  </si>
+  <si>
+    <t xml:space="preserve">home</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trading Details</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Warranty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Delivery Terms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Packaging</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Price Amount</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Price Base Quantity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Minimum Order Quantity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Free Sample</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Warranty Validity Period</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Warranty Information</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Incoterms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Special Terms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estimated Delivery Period</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Applicable Address Country</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transport Mode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Packaging Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Package Quantity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CURRENCY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EUR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">piece</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRUE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CIF (Cost,Insurance and Freight)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">weeks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">China</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sea | Air</t>
+  </si>
+  <si>
+    <t xml:space="preserve">box</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">items</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FALSE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FOB (Free on Board)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Road</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cartons</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DAT (Delivered at Terminal)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">polybag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">working days</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">month</t>
+  </si>
+  <si>
+    <t xml:space="preserve">days</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Turkey</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SEK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spain|France</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Short Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Definition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Note</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Remark</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Preferred Symbol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IEC Category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Attribute Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Type of packaging in accordance with given regulations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STRING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">General recipe resulting from quality requirements for the final product. Examples: waterproof gluing, increase of fire protection category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The cut says whether and which side of a plate has been smoothed by grinding</t>
+  </si>
+  <si>
     <t xml:space="preserve">QUANTITY</t>
   </si>
   <si>
-    <t xml:space="preserve">NUMBER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BOOLEAN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Property Unit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Product_id1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Plastic-head mallet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mallet that can be used mosaic tiling</t>
-  </si>
-  <si>
-    <t xml:space="preserve">83</t>
-  </si>
-  <si>
-    <t xml:space="preserve">43</t>
-  </si>
-  <si>
-    <t xml:space="preserve">315</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RED|GREEN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Product_id2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Iron-head mallet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Strong mallet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">78</t>
-  </si>
-  <si>
-    <t xml:space="preserve">35</t>
-  </si>
-  <si>
-    <t xml:space="preserve">300</t>
-  </si>
-  <si>
-    <t xml:space="preserve">industry</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Product_id3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wood-head mallet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Great for metal working</t>
-  </si>
-  <si>
-    <t xml:space="preserve">80</t>
-  </si>
-  <si>
-    <t xml:space="preserve">40</t>
-  </si>
-  <si>
-    <t xml:space="preserve">320</t>
-  </si>
-  <si>
-    <t xml:space="preserve">home</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Trading Details</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Warranty</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Delivery Terms</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Packaging</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Price Amount</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Price Base Quantity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Minimum Order Quantity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Free Sample</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Warranty Validity Period</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Warranty Information</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Incoterms</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Special Terms</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Estimated Delivery Period</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Applicable Address Country</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Transport Mode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Packaging Type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Package Quantity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AMOUNT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EUR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">piece</t>
-  </si>
-  <si>
-    <t xml:space="preserve">year</t>
-  </si>
-  <si>
-    <t xml:space="preserve">weeks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">items</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TRUE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CIF (Cost,Insurance and Freight)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">China</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sea | Air</t>
-  </si>
-  <si>
-    <t xml:space="preserve">box</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FALSE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FOB (Free on Board)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Road</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cartons</t>
-  </si>
-  <si>
-    <t xml:space="preserve">30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DAT (Delivered at Terminal)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">polybag</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Short Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Definition</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Note</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Remark</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Preferred Symbol</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IEC Category</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Attribute Type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Data Type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Type of packaging in accordance with given regulations</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STRING</t>
-  </si>
-  <si>
-    <t xml:space="preserve">General recipe resulting from quality requirements for the final product. Examples: waterproof gluing, increase of fire protection category</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The cut says whether and which side of a plate has been smoothed by grinding</t>
-  </si>
-  <si>
     <t xml:space="preserve">Characteristic to differentiate between different products of a product family or special variants</t>
   </si>
   <si>
@@ -689,28 +719,10 @@
     <t xml:space="preserve">WarrantyValidity</t>
   </si>
   <si>
-    <t xml:space="preserve">working days</t>
-  </si>
-  <si>
     <t xml:space="preserve">CIP (Carriage and Insurance Paid to)</t>
   </si>
   <si>
-    <t xml:space="preserve">USD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">month</t>
-  </si>
-  <si>
-    <t xml:space="preserve">days</t>
-  </si>
-  <si>
     <t xml:space="preserve">CFR (Cost and Freight)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SEK</t>
   </si>
   <si>
     <t xml:space="preserve">m</t>
@@ -741,12 +753,11 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -774,6 +785,12 @@
       <b val="true"/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -838,7 +855,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -867,11 +884,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -912,8 +937,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="258.102040816326"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="287.127551020408"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="10.8010204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1172,56 +1197,65 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AP7"/>
+  <dimension ref="A1:AX7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AN1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AP6" activeCellId="0" sqref="AP6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AT1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AV6" activeCellId="0" sqref="AV6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="26.7295918367347"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="44.0051020408163"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="24.9744897959184"/>
-    <col collapsed="false" hidden="false" max="7" min="5" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="25.3775510204082"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="63.984693877551"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="50.484693877551"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="29.8316326530612"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="45.8979591836735"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="45.4897959183674"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="24.9744897959184"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="36.3112244897959"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="46.1683673469388"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="39.4183673469388"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="53.4591836734694"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="24.9744897959184"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="46.3010204081633"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="24.9744897959184"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="39.280612244898"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="24.9744897959184"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="34.5561224489796"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="27.1326530612245"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="41.0357142857143"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="38.6071428571429"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="38.7448979591837"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="31.9948979591837"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="29.2908163265306"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="51.8367346938776"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="37.2602040816326"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="34.1530612244898"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="49.9489795918367"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="33.6122448979592"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="36.5816326530612"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="25.3775510204082"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="56.8316326530612"/>
-    <col collapsed="false" hidden="false" max="1025" min="41" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="27.1326530612245"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="44.5459183673469"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="25.2448979591837"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.5969387755102"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="21.5969387755102"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="21.5969387755102"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="25.6479591836735"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="64.6632653061225"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="51.1632653061225"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="30.2397959183673"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="46.4387755102041"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="46.030612244898"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="25.2448979591837"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="36.719387755102"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="46.7091836734694"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="39.8214285714286"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="54.1326530612245"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="25.2448979591837"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="46.8418367346939"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="25.2448979591837"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="39.6887755102041"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="25.2448979591837"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="34.9642857142857"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="27.4030612244898"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="41.5765306122449"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="39.1479591836735"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="39.280612244898"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="32.3979591836735"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="29.6989795918367"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="52.3775510204082"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="37.6632653061224"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="34.5561224489796"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="50.6224489795918"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="34.0204081632653"/>
+    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="36.9897959183673"/>
+    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="21.5969387755102"/>
+    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="25.6479591836735"/>
+    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="45" min="45" style="0" width="21.5969387755102"/>
+    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="47" min="47" style="0" width="57.6428571428571"/>
+    <col collapsed="false" hidden="false" max="48" min="48" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="1025" min="49" style="0" width="10.8010204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0"/>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -1230,12 +1264,12 @@
       </c>
       <c r="F1" s="5"/>
       <c r="G1" s="5"/>
-      <c r="H1" s="5" t="s">
-        <v>49</v>
-      </c>
+      <c r="H1" s="5"/>
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
+      <c r="K1" s="5" t="s">
+        <v>49</v>
+      </c>
       <c r="L1" s="5"/>
       <c r="M1" s="5"/>
       <c r="N1" s="5"/>
@@ -1265,6 +1299,14 @@
       <c r="AL1" s="5"/>
       <c r="AM1" s="5"/>
       <c r="AN1" s="5"/>
+      <c r="AO1" s="5"/>
+      <c r="AP1" s="5"/>
+      <c r="AQ1" s="5"/>
+      <c r="AR1" s="5"/>
+      <c r="AS1" s="5"/>
+      <c r="AT1" s="5"/>
+      <c r="AU1" s="5"/>
+      <c r="AV1" s="5"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
@@ -1282,115 +1324,123 @@
       <c r="E2" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="3"/>
+      <c r="G2" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="H2" s="3"/>
+      <c r="I2" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="J2" s="3"/>
+      <c r="K2" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="L2" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="M2" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="N2" s="3"/>
+      <c r="O2" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="P2" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="Q2" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="N2" s="6" t="s">
+      <c r="R2" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="O2" s="6" t="s">
+      <c r="S2" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="P2" s="6" t="s">
+      <c r="T2" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="Q2" s="6" t="s">
+      <c r="U2" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="R2" s="6" t="s">
+      <c r="V2" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="S2" s="6" t="s">
+      <c r="W2" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="T2" s="6" t="s">
+      <c r="X2" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="U2" s="6" t="s">
+      <c r="Y2" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="V2" s="6" t="s">
+      <c r="Z2" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="W2" s="6" t="s">
+      <c r="AA2" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="X2" s="6" t="s">
+      <c r="AB2" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="Y2" s="6" t="s">
+      <c r="AC2" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="Z2" s="6" t="s">
+      <c r="AD2" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="AA2" s="6" t="s">
+      <c r="AE2" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="AB2" s="6" t="s">
+      <c r="AF2" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="AC2" s="6" t="s">
+      <c r="AG2" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="AD2" s="6" t="s">
+      <c r="AH2" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="AE2" s="6" t="s">
+      <c r="AI2" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="AF2" s="6" t="s">
+      <c r="AJ2" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="AG2" s="6" t="s">
+      <c r="AK2" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="AH2" s="6" t="s">
+      <c r="AL2" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="AI2" s="6" t="s">
+      <c r="AM2" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="AJ2" s="6" t="s">
+      <c r="AN2" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="AK2" s="6" t="s">
+      <c r="AO2" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="AL2" s="6" t="s">
+      <c r="AP2" s="3"/>
+      <c r="AQ2" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="AM2" s="6" t="s">
+      <c r="AR2" s="3"/>
+      <c r="AS2" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="AN2" s="6" t="s">
+      <c r="AT2" s="3"/>
+      <c r="AU2" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="AO2" s="0" t="s">
+      <c r="AV2" s="3"/>
+      <c r="AW2" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="AP2" s="0" t="s">
+      <c r="AX2" s="7" t="s">
         <v>91</v>
       </c>
     </row>
@@ -1411,31 +1461,31 @@
         <v>95</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>95</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="J3" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="M3" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="K3" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>94</v>
-      </c>
       <c r="N3" s="3" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="O3" s="3" t="s">
         <v>94</v>
@@ -1471,76 +1521,94 @@
         <v>94</v>
       </c>
       <c r="Z3" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="AA3" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="AB3" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="AC3" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="AD3" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="AE3" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="AF3" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="AG3" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="AH3" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="AI3" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="AJ3" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="AK3" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="AL3" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="AM3" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="AN3" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="AO3" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="AP3" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="AA3" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="AB3" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="AC3" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="AD3" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="AE3" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="AF3" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="AG3" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="AH3" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="AI3" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="AJ3" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="AK3" s="3" t="s">
+      <c r="AQ3" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="AL3" s="3" t="s">
+      <c r="AR3" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="AS3" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="AM3" s="3" t="s">
+      <c r="AT3" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="AU3" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="AN3" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="AO3" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="AP3" s="0" t="s">
+      <c r="AV3" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="AW3" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="AX3" s="7" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
-      <c r="E4" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>99</v>
-      </c>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
-      <c r="J4" s="4"/>
+      <c r="J4" s="3"/>
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
@@ -1567,33 +1635,47 @@
       <c r="AH4" s="3"/>
       <c r="AI4" s="3"/>
       <c r="AJ4" s="3"/>
-      <c r="AK4" s="4"/>
-      <c r="AL4" s="4"/>
-      <c r="AM4" s="4"/>
-      <c r="AN4" s="4"/>
+      <c r="AK4" s="3"/>
+      <c r="AL4" s="3"/>
+      <c r="AM4" s="3"/>
+      <c r="AN4" s="3"/>
+      <c r="AO4" s="3"/>
+      <c r="AP4" s="3"/>
+      <c r="AQ4" s="3"/>
+      <c r="AR4" s="3"/>
+      <c r="AS4" s="3"/>
+      <c r="AT4" s="3"/>
+      <c r="AU4" s="3"/>
+      <c r="AV4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="9" t="s">
         <v>103</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
+      <c r="H5" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>104</v>
+      </c>
       <c r="K5" s="4"/>
       <c r="L5" s="4"/>
       <c r="M5" s="4"/>
@@ -1614,90 +1696,118 @@
       <c r="AB5" s="4"/>
       <c r="AC5" s="4"/>
       <c r="AD5" s="4"/>
-      <c r="AE5" s="7"/>
-      <c r="AF5" s="7"/>
+      <c r="AE5" s="4"/>
+      <c r="AF5" s="4"/>
       <c r="AG5" s="4"/>
       <c r="AH5" s="4"/>
-      <c r="AI5" s="4"/>
-      <c r="AJ5" s="4"/>
+      <c r="AI5" s="10"/>
+      <c r="AJ5" s="10"/>
       <c r="AK5" s="4"/>
       <c r="AL5" s="4"/>
       <c r="AM5" s="4"/>
       <c r="AN5" s="4"/>
-      <c r="AO5" s="0" t="s">
-        <v>106</v>
+      <c r="AO5" s="4"/>
+      <c r="AP5" s="4"/>
+      <c r="AQ5" s="4"/>
+      <c r="AR5" s="4"/>
+      <c r="AS5" s="4"/>
+      <c r="AT5" s="4"/>
+      <c r="AU5" s="4"/>
+      <c r="AV5" s="4"/>
+      <c r="AW5" s="7" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="C6" s="0" t="s">
+      <c r="B6" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="C6" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="E6" s="0" t="s">
+      <c r="D6" s="7" t="s">
         <v>110</v>
       </c>
+      <c r="E6" s="7" t="s">
+        <v>111</v>
+      </c>
       <c r="F6" s="0" t="s">
-        <v>111</v>
-      </c>
-      <c r="G6" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="G6" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="AP6" s="0" t="s">
+      <c r="H6" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="I6" s="7" t="s">
         <v>113</v>
       </c>
+      <c r="J6" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="AW6" s="7"/>
+      <c r="AX6" s="7" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="0" t="s">
-        <v>114</v>
-      </c>
-      <c r="C7" s="0" t="s">
+      <c r="B7" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="C7" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="E7" s="0" t="s">
+      <c r="D7" s="7" t="s">
         <v>117</v>
       </c>
+      <c r="E7" s="7" t="s">
+        <v>118</v>
+      </c>
       <c r="F7" s="0" t="s">
-        <v>118</v>
-      </c>
-      <c r="G7" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="G7" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="AP7" s="0" t="s">
+      <c r="H7" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="I7" s="7" t="s">
         <v>120</v>
+      </c>
+      <c r="J7" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="AW7" s="7"/>
+      <c r="AX7" s="7" t="s">
+        <v>121</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="H1:AN1"/>
+    <mergeCell ref="E1:J1"/>
+    <mergeCell ref="K1:AV1"/>
   </mergeCells>
   <dataValidations count="5">
-    <dataValidation allowBlank="true" error="Please, select one of the available options" errorTitle="Invalid input !" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="AE5" type="list">
+    <dataValidation allowBlank="true" error="Please, select one of the available options" errorTitle="Invalid input !" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F5" type="list">
+      <formula1>Dimension</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" error="Please, select one of the available options" errorTitle="Invalid input !" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H5" type="list">
+      <formula1>Dimension</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" error="Please, select one of the available options" errorTitle="Invalid input !" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J5" type="list">
+      <formula1>Dimension</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" error="Please, select one of the available options" errorTitle="Invalid input !" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="AI5" type="list">
       <formula1>Boolean</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" error="Please, select one of the available options" errorTitle="Invalid input !" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="AF5" type="list">
+    <dataValidation allowBlank="true" error="Please, select one of the available options" errorTitle="Invalid input !" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="AJ5" type="list">
       <formula1>Boolean</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" error="Please, select one of the available options" errorTitle="Invalid input !" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E4" type="list">
-      <formula1>Dimension</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" error="Please, select one of the available options" errorTitle="Invalid input !" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F4" type="list">
-      <formula1>Dimension</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" error="Please, select one of the available options" errorTitle="Invalid input !" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G4" type="list">
-      <formula1>Dimension</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -1716,71 +1826,80 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AN7"/>
+  <dimension ref="A1:AV7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="26.7295918367347"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="44.0051020408163"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.9744897959184"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="43.7397959183673"/>
-    <col collapsed="false" hidden="false" max="7" min="5" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="25.3775510204082"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="63.984693877551"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="50.484693877551"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="29.8316326530612"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="45.8979591836735"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="45.4897959183674"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="24.9744897959184"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="36.3112244897959"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="46.1683673469388"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="39.4183673469388"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="53.4591836734694"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="24.9744897959184"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="46.3010204081633"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="24.9744897959184"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="39.280612244898"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="24.9744897959184"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="34.5561224489796"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="27.1326530612245"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="41.0357142857143"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="38.6071428571429"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="38.7448979591837"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="31.9948979591837"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="29.2908163265306"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="51.8367346938776"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="37.2602040816326"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="34.1530612244898"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="49.9489795918367"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="33.6122448979592"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="36.5816326530612"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="25.3775510204082"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="56.8316326530612"/>
-    <col collapsed="false" hidden="false" max="1025" min="41" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="27.1326530612245"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="44.5459183673469"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.2448979591837"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="44.2755102040816"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.5969387755102"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="21.5969387755102"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="21.5969387755102"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="25.6479591836735"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="64.6632653061225"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="51.1632653061225"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="30.2397959183673"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="46.4387755102041"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="46.030612244898"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="25.2448979591837"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="36.719387755102"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="46.7091836734694"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="39.8214285714286"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="54.1326530612245"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="25.2448979591837"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="46.8418367346939"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="25.2448979591837"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="39.6887755102041"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="25.2448979591837"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="34.9642857142857"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="27.4030612244898"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="41.5765306122449"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="39.1479591836735"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="39.280612244898"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="32.3979591836735"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="29.6989795918367"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="52.3775510204082"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="37.6632653061224"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="34.5561224489796"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="50.6224489795918"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="34.0204081632653"/>
+    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="36.9897959183673"/>
+    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="21.5969387755102"/>
+    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="25.6479591836735"/>
+    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="45" min="45" style="0" width="21.5969387755102"/>
+    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="47" min="47" style="0" width="57.6428571428571"/>
+    <col collapsed="false" hidden="false" max="48" min="48" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="1025" min="49" style="0" width="10.8010204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0"/>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8" t="s">
+      <c r="E1" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="G1" s="8"/>
-      <c r="H1" s="5" t="s">
-        <v>49</v>
-      </c>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
+      <c r="K1" s="5" t="s">
+        <v>49</v>
+      </c>
       <c r="L1" s="5"/>
       <c r="M1" s="5"/>
       <c r="N1" s="5"/>
@@ -1810,6 +1929,14 @@
       <c r="AL1" s="5"/>
       <c r="AM1" s="5"/>
       <c r="AN1" s="5"/>
+      <c r="AO1" s="5"/>
+      <c r="AP1" s="5"/>
+      <c r="AQ1" s="5"/>
+      <c r="AR1" s="5"/>
+      <c r="AS1" s="5"/>
+      <c r="AT1" s="5"/>
+      <c r="AU1" s="5"/>
+      <c r="AV1" s="5"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
@@ -1827,111 +1954,119 @@
       <c r="E2" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="3"/>
+      <c r="G2" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="H2" s="3"/>
+      <c r="I2" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="J2" s="3"/>
+      <c r="K2" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="L2" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="M2" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="N2" s="3"/>
+      <c r="O2" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="P2" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="Q2" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="N2" s="6" t="s">
+      <c r="R2" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="O2" s="6" t="s">
+      <c r="S2" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="P2" s="6" t="s">
+      <c r="T2" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="Q2" s="6" t="s">
+      <c r="U2" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="R2" s="6" t="s">
+      <c r="V2" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="S2" s="6" t="s">
+      <c r="W2" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="T2" s="6" t="s">
+      <c r="X2" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="U2" s="6" t="s">
+      <c r="Y2" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="V2" s="6" t="s">
+      <c r="Z2" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="W2" s="6" t="s">
+      <c r="AA2" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="X2" s="6" t="s">
+      <c r="AB2" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="Y2" s="6" t="s">
+      <c r="AC2" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="Z2" s="6" t="s">
+      <c r="AD2" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="AA2" s="6" t="s">
+      <c r="AE2" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="AB2" s="6" t="s">
+      <c r="AF2" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="AC2" s="6" t="s">
+      <c r="AG2" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="AD2" s="6" t="s">
+      <c r="AH2" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="AE2" s="6" t="s">
+      <c r="AI2" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="AF2" s="6" t="s">
+      <c r="AJ2" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="AG2" s="6" t="s">
+      <c r="AK2" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="AH2" s="6" t="s">
+      <c r="AL2" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="AI2" s="6" t="s">
+      <c r="AM2" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="AJ2" s="6" t="s">
+      <c r="AN2" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="AK2" s="6" t="s">
+      <c r="AO2" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="AL2" s="6" t="s">
+      <c r="AP2" s="3"/>
+      <c r="AQ2" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="AM2" s="6" t="s">
+      <c r="AR2" s="3"/>
+      <c r="AS2" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="AN2" s="6" t="s">
+      <c r="AT2" s="3"/>
+      <c r="AU2" s="6" t="s">
         <v>89</v>
       </c>
+      <c r="AV2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
@@ -1950,31 +2085,31 @@
         <v>95</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>95</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="J3" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="M3" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="K3" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>94</v>
-      </c>
       <c r="N3" s="3" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="O3" s="3" t="s">
         <v>94</v>
@@ -2010,70 +2145,88 @@
         <v>94</v>
       </c>
       <c r="Z3" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="AA3" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="AB3" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="AC3" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="AD3" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="AE3" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="AF3" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="AG3" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="AH3" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="AI3" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="AJ3" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="AK3" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="AL3" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="AM3" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="AN3" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="AO3" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="AP3" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="AA3" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="AB3" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="AC3" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="AD3" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="AE3" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="AF3" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="AG3" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="AH3" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="AI3" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="AJ3" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="AK3" s="3" t="s">
+      <c r="AQ3" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="AL3" s="3" t="s">
+      <c r="AR3" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="AS3" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="AM3" s="3" t="s">
+      <c r="AT3" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="AU3" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="AN3" s="3" t="s">
-        <v>95</v>
+      <c r="AV3" s="3" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
-      <c r="E4" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>99</v>
-      </c>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
-      <c r="J4" s="4"/>
+      <c r="J4" s="3"/>
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
@@ -2100,10 +2253,18 @@
       <c r="AH4" s="3"/>
       <c r="AI4" s="3"/>
       <c r="AJ4" s="3"/>
-      <c r="AK4" s="4"/>
-      <c r="AL4" s="4"/>
-      <c r="AM4" s="4"/>
-      <c r="AN4" s="4"/>
+      <c r="AK4" s="3"/>
+      <c r="AL4" s="3"/>
+      <c r="AM4" s="3"/>
+      <c r="AN4" s="3"/>
+      <c r="AO4" s="3"/>
+      <c r="AP4" s="3"/>
+      <c r="AQ4" s="3"/>
+      <c r="AR4" s="3"/>
+      <c r="AS4" s="3"/>
+      <c r="AT4" s="3"/>
+      <c r="AU4" s="3"/>
+      <c r="AV4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="2" t="s">
@@ -2116,17 +2277,23 @@
         <v>102</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>103</v>
+        <v>122</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>104</v>
+        <v>123</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
+        <v>124</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>123</v>
+      </c>
       <c r="K5" s="4"/>
       <c r="L5" s="4"/>
       <c r="M5" s="4"/>
@@ -2147,80 +2314,106 @@
       <c r="AB5" s="4"/>
       <c r="AC5" s="4"/>
       <c r="AD5" s="4"/>
-      <c r="AE5" s="7"/>
-      <c r="AF5" s="7"/>
+      <c r="AE5" s="4"/>
+      <c r="AF5" s="4"/>
       <c r="AG5" s="4"/>
       <c r="AH5" s="4"/>
-      <c r="AI5" s="4"/>
-      <c r="AJ5" s="4"/>
+      <c r="AI5" s="10"/>
+      <c r="AJ5" s="10"/>
       <c r="AK5" s="4"/>
       <c r="AL5" s="4"/>
       <c r="AM5" s="4"/>
       <c r="AN5" s="4"/>
+      <c r="AO5" s="4"/>
+      <c r="AP5" s="4"/>
+      <c r="AQ5" s="4"/>
+      <c r="AR5" s="4"/>
+      <c r="AS5" s="4"/>
+      <c r="AT5" s="4"/>
+      <c r="AU5" s="4"/>
+      <c r="AV5" s="4"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>111</v>
+        <v>123</v>
       </c>
       <c r="G6" s="0" t="s">
         <v>112</v>
       </c>
+      <c r="H6" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="I6" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="J6" s="0" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
       <c r="G7" s="0" t="s">
         <v>119</v>
       </c>
+      <c r="H7" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="I7" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="J7" s="0" t="s">
+        <v>104</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="H1:AN1"/>
+    <mergeCell ref="E1:J1"/>
+    <mergeCell ref="K1:AV1"/>
   </mergeCells>
   <dataValidations count="5">
-    <dataValidation allowBlank="true" error="Please, select one of the available options" errorTitle="Invalid input !" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E4" type="list">
+    <dataValidation allowBlank="true" error="Please, select one of the available options" errorTitle="Invalid input !" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F5" type="list">
       <formula1>Dimension</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" error="Please, select one of the available options" errorTitle="Invalid input !" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F4" type="list">
+    <dataValidation allowBlank="true" error="Please, select one of the available options" errorTitle="Invalid input !" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H5" type="list">
       <formula1>Dimension</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" error="Please, select one of the available options" errorTitle="Invalid input !" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G4" type="list">
+    <dataValidation allowBlank="true" error="Please, select one of the available options" errorTitle="Invalid input !" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J5" type="list">
       <formula1>Dimension</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" error="Please, select one of the available options" errorTitle="Invalid input !" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="AE5" type="list">
+    <dataValidation allowBlank="true" error="Please, select one of the available options" errorTitle="Invalid input !" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="AI5" type="list">
       <formula1>Boolean</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" error="Please, select one of the available options" errorTitle="Invalid input !" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="AF5" type="list">
+    <dataValidation allowBlank="true" error="Please, select one of the available options" errorTitle="Invalid input !" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="AJ5" type="list">
       <formula1>Boolean</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -2240,55 +2433,66 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O7"/>
+  <dimension ref="A1:U7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="P1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="U8" activeCellId="0" sqref="U8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="26.7295918367347"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="44.0051020408163"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.2704081632653"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="33.75"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="33.6122448979592"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="29.6989795918367"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="35.0969387755102"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="37.5255102040816"/>
-    <col collapsed="false" hidden="false" max="14" min="13" style="0" width="22.0051020408163"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="24.4336734693878"/>
-    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="27.1326530612245"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="44.5459183673469"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.5969387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="34.1530612244898"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="34.0204081632653"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="30.1020408163265"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="35.6377551020408"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="37.9336734693878"/>
+    <col collapsed="false" hidden="false" max="19" min="18" style="0" width="22.2755102040816"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="24.7040816326531"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="10.8010204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0"/>
       <c r="B1" s="3"/>
       <c r="C1" s="5" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
-      <c r="G1" s="5" t="s">
-        <v>122</v>
-      </c>
+      <c r="G1" s="5"/>
       <c r="H1" s="5"/>
-      <c r="I1" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="J1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5" t="s">
+        <v>127</v>
+      </c>
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5" t="s">
-        <v>124</v>
-      </c>
+      <c r="M1" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="N1" s="5"/>
       <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5"/>
+      <c r="S1" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="T1" s="5"/>
+      <c r="U1" s="5"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
@@ -2298,44 +2502,50 @@
         <v>51</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>126</v>
-      </c>
+        <v>130</v>
+      </c>
+      <c r="D2" s="3"/>
       <c r="E2" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>128</v>
-      </c>
+        <v>131</v>
+      </c>
+      <c r="F2" s="3"/>
       <c r="G2" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>130</v>
-      </c>
+        <v>132</v>
+      </c>
+      <c r="H2" s="3"/>
       <c r="I2" s="6" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>133</v>
-      </c>
+        <v>134</v>
+      </c>
+      <c r="K2" s="3"/>
       <c r="L2" s="6" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="N2" s="6" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="O2" s="6" t="s">
-        <v>137</v>
-      </c>
+        <v>138</v>
+      </c>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="R2" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="S2" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="T2" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="U2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
@@ -2345,31 +2555,31 @@
         <v>93</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>138</v>
+        <v>95</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>95</v>
+        <v>143</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>95</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>95</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="L3" s="3" t="s">
         <v>93</v>
@@ -2383,174 +2593,240 @@
       <c r="O3" s="3" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="P3" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="S3" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="T3" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="U3" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B4" s="3"/>
-      <c r="C4" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>140</v>
-      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
       <c r="F4" s="3"/>
-      <c r="G4" s="4" t="s">
-        <v>141</v>
-      </c>
+      <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
-      <c r="K4" s="4" t="s">
-        <v>142</v>
-      </c>
+      <c r="K4" s="3"/>
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
-      <c r="O4" s="4" t="s">
-        <v>143</v>
-      </c>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="E5" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="F5" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="G5" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="H5" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="J5" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="J5" s="4"/>
       <c r="K5" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="L5" s="4"/>
+      <c r="M5" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="N5" s="4"/>
+      <c r="O5" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="L5" s="4" t="s">
+      <c r="P5" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q5" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="R5" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="S5" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="T5" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="U5" s="4" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="K6" s="0" t="s">
         <v>149</v>
       </c>
-      <c r="M5" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="N5" s="4" t="s">
+      <c r="M6" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="O6" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="P6" s="0" t="s">
         <v>151</v>
       </c>
-      <c r="O5" s="4" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>153</v>
-      </c>
-      <c r="D6" s="0" t="s">
+      <c r="R6" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="S6" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="T6" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="U6" s="0" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C7" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="E6" s="0" t="s">
+      <c r="D7" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="F7" s="0" t="s">
         <v>146</v>
       </c>
-      <c r="F6" s="0" t="s">
-        <v>154</v>
-      </c>
-      <c r="G6" s="0" t="s">
-        <v>155</v>
-      </c>
-      <c r="I6" s="0" t="s">
+      <c r="G7" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="K7" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="M7" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="O7" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="P7" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="R7" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="S7" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="T7" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="U7" s="0" t="s">
         <v>156</v>
-      </c>
-      <c r="K6" s="0" t="s">
-        <v>144</v>
-      </c>
-      <c r="M6" s="0" t="s">
-        <v>157</v>
-      </c>
-      <c r="N6" s="0" t="s">
-        <v>158</v>
-      </c>
-      <c r="O6" s="0" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="0" t="s">
-        <v>114</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>145</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>145</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>160</v>
-      </c>
-      <c r="F7" s="0" t="s">
-        <v>154</v>
-      </c>
-      <c r="G7" s="0" t="s">
-        <v>161</v>
-      </c>
-      <c r="I7" s="0" t="s">
-        <v>162</v>
-      </c>
-      <c r="K7" s="0" t="s">
-        <v>161</v>
-      </c>
-      <c r="M7" s="0" t="s">
-        <v>157</v>
-      </c>
-      <c r="N7" s="0" t="s">
-        <v>163</v>
-      </c>
-      <c r="O7" s="0" t="s">
-        <v>145</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="C1:F1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="I1:M1"/>
-    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="C1:I1"/>
+    <mergeCell ref="J1:L1"/>
+    <mergeCell ref="M1:R1"/>
+    <mergeCell ref="S1:U1"/>
   </mergeCells>
   <dataValidations count="5">
-    <dataValidation allowBlank="true" error="Please, select one of the available options" errorTitle="Invalid input !" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C4" type="list">
+    <dataValidation allowBlank="true" error="Please, select one of the available options" errorTitle="Invalid input !" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D5" type="list">
       <formula1>Currency</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" error="Please, select one of the available options" errorTitle="Invalid input !" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F5" type="list">
+    <dataValidation allowBlank="true" error="Please, select one of the available options" errorTitle="Invalid input !" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K5" type="list">
+      <formula1>WarrantyValidity</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" error="Please, select one of the available options" errorTitle="Invalid input !" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="P5" type="list">
+      <formula1>DeliveryPeriod</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" error="Please, select one of the available options" errorTitle="Invalid input !" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I5" type="list">
       <formula1>Boolean</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" error="Please, select one of the available options" errorTitle="Invalid input !" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G4" type="list">
+    <dataValidation allowBlank="true" error="Please, select one of the available options" errorTitle="Invalid input !" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="M5" type="list">
       <formula1>WarrantyValidity</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" error="Please, select one of the available options" errorTitle="Invalid input !" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I5" type="list">
-      <formula1>Incoterms</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" error="Please, select one of the available options" errorTitle="Invalid input !" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K4" type="list">
-      <formula1>DeliveryPeriod</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -2569,55 +2845,66 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O7"/>
+  <dimension ref="A1:U7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O4" activeCellId="0" sqref="O4"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="26.7295918367347"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="44.0051020408163"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.2704081632653"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="33.75"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="33.6122448979592"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="29.6989795918367"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="38.3367346938776"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="35.0969387755102"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="37.5255102040816"/>
-    <col collapsed="false" hidden="false" max="14" min="13" style="0" width="22.0051020408163"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="24.4336734693878"/>
-    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="27.1326530612245"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="44.5459183673469"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.5969387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="34.1530612244898"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="34.0204081632653"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="30.1020408163265"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="38.8775510204082"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="35.6377551020408"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="37.9336734693878"/>
+    <col collapsed="false" hidden="false" max="19" min="18" style="0" width="22.2755102040816"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="24.7040816326531"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="10.8010204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0"/>
       <c r="B1" s="3"/>
       <c r="C1" s="5" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
-      <c r="G1" s="5" t="s">
-        <v>122</v>
-      </c>
+      <c r="G1" s="5"/>
       <c r="H1" s="5"/>
-      <c r="I1" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="J1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5" t="s">
+        <v>127</v>
+      </c>
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5" t="s">
-        <v>124</v>
-      </c>
+      <c r="M1" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="N1" s="5"/>
       <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5"/>
+      <c r="S1" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="T1" s="5"/>
+      <c r="U1" s="5"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
@@ -2627,44 +2914,50 @@
         <v>51</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>126</v>
-      </c>
+        <v>130</v>
+      </c>
+      <c r="D2" s="3"/>
       <c r="E2" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>128</v>
-      </c>
+        <v>131</v>
+      </c>
+      <c r="F2" s="3"/>
       <c r="G2" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>130</v>
-      </c>
+        <v>132</v>
+      </c>
+      <c r="H2" s="3"/>
       <c r="I2" s="6" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>133</v>
-      </c>
+        <v>134</v>
+      </c>
+      <c r="K2" s="3"/>
       <c r="L2" s="6" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="N2" s="6" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="O2" s="6" t="s">
-        <v>137</v>
-      </c>
+        <v>138</v>
+      </c>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="R2" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="S2" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="T2" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="U2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
@@ -2677,28 +2970,28 @@
         <v>95</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>95</v>
+        <v>143</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>95</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>95</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="L3" s="3" t="s">
         <v>93</v>
@@ -2712,173 +3005,245 @@
       <c r="O3" s="3" t="s">
         <v>95</v>
       </c>
+      <c r="P3" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="S3" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="T3" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="U3" s="3" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B4" s="3"/>
-      <c r="C4" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>140</v>
-      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
       <c r="F4" s="3"/>
-      <c r="G4" s="4" t="s">
-        <v>141</v>
-      </c>
+      <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
-      <c r="K4" s="4" t="s">
-        <v>142</v>
-      </c>
+      <c r="K4" s="3"/>
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
-      <c r="O4" s="4" t="s">
-        <v>143</v>
-      </c>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="2" t="s">
         <v>100</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="E5" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="F5" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="G5" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="G5" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="H5" s="4"/>
+      <c r="H5" s="4" t="s">
+        <v>146</v>
+      </c>
       <c r="I5" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="J5" s="4"/>
+      <c r="J5" s="4" t="s">
+        <v>145</v>
+      </c>
       <c r="K5" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="L5" s="4" t="s">
         <v>149</v>
       </c>
+      <c r="L5" s="4"/>
       <c r="M5" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="N5" s="4" t="s">
-        <v>151</v>
-      </c>
+      <c r="N5" s="4"/>
       <c r="O5" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="P5" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="Q5" s="4" t="s">
         <v>152</v>
+      </c>
+      <c r="R5" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="S5" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="T5" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="U5" s="4" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="D6" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="E6" s="0" t="s">
         <v>145</v>
       </c>
-      <c r="E6" s="0" t="s">
+      <c r="F6" s="0" t="s">
         <v>146</v>
       </c>
-      <c r="F6" s="0" t="s">
-        <v>154</v>
-      </c>
       <c r="G6" s="0" t="s">
-        <v>155</v>
+        <v>147</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>146</v>
       </c>
       <c r="I6" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="J6" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="K6" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="M6" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="O6" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="P6" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="Q6" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="R6" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="S6" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="T6" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="U6" s="0" t="s">
         <v>156</v>
-      </c>
-      <c r="K6" s="0" t="s">
-        <v>144</v>
-      </c>
-      <c r="M6" s="0" t="s">
-        <v>157</v>
-      </c>
-      <c r="N6" s="0" t="s">
-        <v>158</v>
-      </c>
-      <c r="O6" s="0" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>145</v>
       </c>
       <c r="D7" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="E7" s="0" t="s">
         <v>145</v>
       </c>
-      <c r="E7" s="0" t="s">
+      <c r="F7" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="I7" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="J7" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="K7" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="M7" s="0" t="s">
+        <v>164</v>
+      </c>
+      <c r="O7" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="P7" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q7" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="R7" s="0" t="s">
         <v>160</v>
       </c>
-      <c r="F7" s="0" t="s">
-        <v>154</v>
-      </c>
-      <c r="G7" s="0" t="s">
-        <v>161</v>
-      </c>
-      <c r="I7" s="0" t="s">
-        <v>162</v>
-      </c>
-      <c r="K7" s="0" t="s">
-        <v>161</v>
-      </c>
-      <c r="M7" s="0" t="s">
-        <v>157</v>
-      </c>
-      <c r="N7" s="0" t="s">
-        <v>163</v>
-      </c>
-      <c r="O7" s="0" t="s">
+      <c r="S7" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="T7" s="0" t="s">
         <v>145</v>
+      </c>
+      <c r="U7" s="0" t="s">
+        <v>156</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="C1:F1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="I1:M1"/>
-    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="C1:I1"/>
+    <mergeCell ref="J1:L1"/>
+    <mergeCell ref="M1:R1"/>
+    <mergeCell ref="S1:U1"/>
   </mergeCells>
   <dataValidations count="5">
-    <dataValidation allowBlank="true" error="Please, select one of the available options" errorTitle="Invalid input !" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C4" type="list">
+    <dataValidation allowBlank="true" error="Please, select one of the available options" errorTitle="Invalid input !" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D5" type="list">
       <formula1>Currency</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" error="Please, select one of the available options" errorTitle="Invalid input !" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F5" type="list">
+    <dataValidation allowBlank="true" error="Please, select one of the available options" errorTitle="Invalid input !" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I5" type="list">
       <formula1>Boolean</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" error="Please, select one of the available options" errorTitle="Invalid input !" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G4" type="list">
+    <dataValidation allowBlank="true" error="Please, select one of the available options" errorTitle="Invalid input !" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K5" type="list">
       <formula1>WarrantyValidity</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" error="Please, select one of the available options" errorTitle="Invalid input !" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I5" type="list">
+    <dataValidation allowBlank="true" error="Please, select one of the available options" errorTitle="Invalid input !" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="M5" type="list">
       <formula1>Incoterms</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" error="Please, select one of the available options" errorTitle="Invalid input !" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K4" type="list">
+    <dataValidation allowBlank="true" error="Please, select one of the available options" errorTitle="Invalid input !" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="P5" type="list">
       <formula1>DeliveryPeriod</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -2906,494 +3271,494 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.9030612244898"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="56.0204081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="62.7704081632653"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="7.56122448979592"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="62.7704081632653"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.3010204081633"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="6.75"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="20.25"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="14.4438775510204"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="56.6989795918367"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="63.5816326530612"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="63.5816326530612"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="20.5204081632653"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="14.7142857142857"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="10.8010204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="9"/>
-      <c r="B1" s="9" t="s">
+      <c r="A1" s="11"/>
+      <c r="B1" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="C1" s="9" t="s">
-        <v>164</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>165</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>166</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>167</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>168</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>169</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>170</v>
-      </c>
-      <c r="J1" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="K1" s="9" t="s">
-        <v>172</v>
+      <c r="C1" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>176</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>178</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>179</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="K1" s="11" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="12" t="s">
         <v>49</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="D2" s="11" t="s">
-        <v>173</v>
-      </c>
-      <c r="F2" s="11"/>
+      <c r="D2" s="13" t="s">
+        <v>182</v>
+      </c>
+      <c r="F2" s="13"/>
       <c r="K2" s="0" t="s">
-        <v>174</v>
+        <v>183</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="10"/>
+      <c r="A3" s="12"/>
       <c r="B3" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="D3" s="11" t="s">
-        <v>175</v>
-      </c>
-      <c r="F3" s="11"/>
+      <c r="D3" s="13" t="s">
+        <v>184</v>
+      </c>
+      <c r="F3" s="13"/>
       <c r="K3" s="0" t="s">
-        <v>174</v>
+        <v>183</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="10"/>
+      <c r="A4" s="12"/>
       <c r="B4" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="D4" s="11" t="s">
-        <v>176</v>
-      </c>
-      <c r="F4" s="11"/>
+      <c r="D4" s="13" t="s">
+        <v>185</v>
+      </c>
+      <c r="F4" s="13"/>
       <c r="K4" s="0" t="s">
-        <v>95</v>
+        <v>186</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="10"/>
+      <c r="A5" s="12"/>
       <c r="B5" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="D5" s="11" t="s">
-        <v>177</v>
-      </c>
-      <c r="F5" s="11"/>
+      <c r="D5" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="F5" s="13"/>
       <c r="K5" s="0" t="s">
-        <v>174</v>
+        <v>183</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="10"/>
+      <c r="A6" s="12"/>
       <c r="B6" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="D6" s="11" t="s">
-        <v>178</v>
-      </c>
-      <c r="F6" s="11"/>
+      <c r="D6" s="13" t="s">
+        <v>188</v>
+      </c>
+      <c r="F6" s="13"/>
       <c r="K6" s="0" t="s">
-        <v>174</v>
+        <v>183</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="10"/>
+      <c r="A7" s="12"/>
       <c r="B7" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="D7" s="11" t="s">
-        <v>179</v>
-      </c>
-      <c r="F7" s="11"/>
+      <c r="D7" s="13" t="s">
+        <v>189</v>
+      </c>
+      <c r="F7" s="13"/>
       <c r="K7" s="0" t="s">
-        <v>174</v>
+        <v>183</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="10"/>
+      <c r="A8" s="12"/>
       <c r="B8" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="D8" s="11" t="s">
-        <v>177</v>
-      </c>
-      <c r="F8" s="11"/>
+      <c r="D8" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="F8" s="13"/>
       <c r="K8" s="0" t="s">
-        <v>174</v>
+        <v>183</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="10"/>
+      <c r="A9" s="12"/>
       <c r="B9" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="D9" s="11" t="s">
-        <v>180</v>
-      </c>
-      <c r="F9" s="11"/>
+      <c r="D9" s="13" t="s">
+        <v>190</v>
+      </c>
+      <c r="F9" s="13"/>
       <c r="K9" s="0" t="s">
-        <v>174</v>
+        <v>183</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="10"/>
+      <c r="A10" s="12"/>
       <c r="B10" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="D10" s="11" t="s">
-        <v>181</v>
-      </c>
-      <c r="F10" s="11"/>
+      <c r="D10" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="F10" s="13"/>
       <c r="K10" s="0" t="s">
-        <v>174</v>
+        <v>183</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="10"/>
+      <c r="A11" s="12"/>
       <c r="B11" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="D11" s="11" t="s">
-        <v>181</v>
-      </c>
-      <c r="F11" s="11"/>
+      <c r="D11" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="F11" s="13"/>
       <c r="K11" s="0" t="s">
-        <v>174</v>
+        <v>183</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="10"/>
+      <c r="A12" s="12"/>
       <c r="B12" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="D12" s="11" t="s">
-        <v>182</v>
-      </c>
-      <c r="F12" s="11" t="s">
+      <c r="D12" s="13" t="s">
+        <v>192</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>193</v>
+      </c>
+      <c r="K12" s="0" t="s">
         <v>183</v>
       </c>
-      <c r="K12" s="0" t="s">
-        <v>174</v>
-      </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="10"/>
+      <c r="A13" s="12"/>
       <c r="B13" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="D13" s="11" t="s">
-        <v>184</v>
-      </c>
-      <c r="F13" s="11" t="s">
-        <v>185</v>
+      <c r="D13" s="13" t="s">
+        <v>194</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>195</v>
       </c>
       <c r="K13" s="0" t="s">
-        <v>174</v>
+        <v>183</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="10"/>
+      <c r="A14" s="12"/>
       <c r="B14" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="D14" s="11" t="s">
-        <v>186</v>
-      </c>
-      <c r="F14" s="11" t="s">
-        <v>187</v>
+      <c r="D14" s="13" t="s">
+        <v>196</v>
+      </c>
+      <c r="F14" s="13" t="s">
+        <v>197</v>
       </c>
       <c r="K14" s="0" t="s">
-        <v>174</v>
+        <v>183</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="10"/>
+      <c r="A15" s="12"/>
       <c r="B15" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="D15" s="11" t="s">
-        <v>188</v>
-      </c>
-      <c r="F15" s="11"/>
+      <c r="D15" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="F15" s="13"/>
       <c r="K15" s="0" t="s">
-        <v>174</v>
+        <v>183</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="10"/>
+      <c r="A16" s="12"/>
       <c r="B16" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="D16" s="11" t="s">
-        <v>189</v>
-      </c>
-      <c r="F16" s="11"/>
+      <c r="D16" s="13" t="s">
+        <v>199</v>
+      </c>
+      <c r="F16" s="13"/>
       <c r="K16" s="0" t="s">
-        <v>174</v>
+        <v>183</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="10"/>
+      <c r="A17" s="12"/>
       <c r="B17" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="D17" s="11" t="s">
-        <v>190</v>
-      </c>
-      <c r="F17" s="11" t="s">
-        <v>191</v>
+      <c r="D17" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="F17" s="13" t="s">
+        <v>201</v>
       </c>
       <c r="K17" s="0" t="s">
-        <v>174</v>
+        <v>183</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="10"/>
+      <c r="A18" s="12"/>
       <c r="B18" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="D18" s="11" t="s">
-        <v>192</v>
-      </c>
-      <c r="F18" s="11"/>
+      <c r="D18" s="13" t="s">
+        <v>202</v>
+      </c>
+      <c r="F18" s="13"/>
       <c r="K18" s="0" t="s">
-        <v>174</v>
+        <v>183</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="10"/>
+      <c r="A19" s="12"/>
       <c r="B19" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="D19" s="11" t="s">
-        <v>193</v>
-      </c>
-      <c r="F19" s="11" t="s">
-        <v>194</v>
+      <c r="D19" s="13" t="s">
+        <v>203</v>
+      </c>
+      <c r="F19" s="13" t="s">
+        <v>204</v>
       </c>
       <c r="K19" s="0" t="s">
-        <v>174</v>
+        <v>183</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="10"/>
+      <c r="A20" s="12"/>
       <c r="B20" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="D20" s="11" t="s">
-        <v>195</v>
-      </c>
-      <c r="F20" s="11"/>
+      <c r="D20" s="13" t="s">
+        <v>205</v>
+      </c>
+      <c r="F20" s="13"/>
       <c r="K20" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="10"/>
+      <c r="A21" s="12"/>
       <c r="B21" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="D21" s="11" t="s">
-        <v>179</v>
-      </c>
-      <c r="F21" s="11"/>
+      <c r="D21" s="13" t="s">
+        <v>189</v>
+      </c>
+      <c r="F21" s="13"/>
       <c r="K21" s="0" t="s">
-        <v>174</v>
+        <v>183</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="10"/>
+      <c r="A22" s="12"/>
       <c r="B22" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="D22" s="11" t="s">
-        <v>196</v>
-      </c>
-      <c r="F22" s="11"/>
+      <c r="D22" s="13" t="s">
+        <v>206</v>
+      </c>
+      <c r="F22" s="13"/>
       <c r="K22" s="0" t="s">
-        <v>174</v>
+        <v>183</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="10"/>
+      <c r="A23" s="12"/>
       <c r="B23" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="D23" s="11" t="s">
-        <v>197</v>
-      </c>
-      <c r="F23" s="11"/>
+      <c r="D23" s="13" t="s">
+        <v>207</v>
+      </c>
+      <c r="F23" s="13"/>
       <c r="K23" s="0" t="s">
-        <v>174</v>
+        <v>183</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="10"/>
+      <c r="A24" s="12"/>
       <c r="B24" s="0" t="s">
         <v>79</v>
       </c>
-      <c r="D24" s="11" t="s">
-        <v>198</v>
-      </c>
-      <c r="F24" s="11"/>
+      <c r="D24" s="13" t="s">
+        <v>208</v>
+      </c>
+      <c r="F24" s="13"/>
       <c r="K24" s="0" t="s">
-        <v>174</v>
+        <v>183</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="10"/>
+      <c r="A25" s="12"/>
       <c r="B25" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="D25" s="11" t="s">
-        <v>199</v>
-      </c>
-      <c r="F25" s="11"/>
+      <c r="D25" s="13" t="s">
+        <v>209</v>
+      </c>
+      <c r="F25" s="13"/>
       <c r="K25" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="10"/>
+      <c r="A26" s="12"/>
       <c r="B26" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="D26" s="11" t="s">
-        <v>200</v>
-      </c>
-      <c r="F26" s="11"/>
+      <c r="D26" s="13" t="s">
+        <v>210</v>
+      </c>
+      <c r="F26" s="13"/>
       <c r="K26" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="10"/>
+      <c r="A27" s="12"/>
       <c r="B27" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="D27" s="11" t="s">
-        <v>201</v>
-      </c>
-      <c r="F27" s="11"/>
+      <c r="D27" s="13" t="s">
+        <v>211</v>
+      </c>
+      <c r="F27" s="13"/>
       <c r="K27" s="0" t="s">
-        <v>174</v>
+        <v>183</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="10"/>
+      <c r="A28" s="12"/>
       <c r="B28" s="0" t="s">
         <v>83</v>
       </c>
-      <c r="D28" s="11" t="s">
-        <v>202</v>
-      </c>
-      <c r="F28" s="11"/>
+      <c r="D28" s="13" t="s">
+        <v>212</v>
+      </c>
+      <c r="F28" s="13"/>
       <c r="K28" s="0" t="s">
-        <v>174</v>
+        <v>183</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="10"/>
+      <c r="A29" s="12"/>
       <c r="B29" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="D29" s="11" t="s">
-        <v>203</v>
-      </c>
-      <c r="F29" s="11"/>
+      <c r="D29" s="13" t="s">
+        <v>213</v>
+      </c>
+      <c r="F29" s="13"/>
       <c r="K29" s="0" t="s">
-        <v>174</v>
+        <v>183</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="10"/>
+      <c r="A30" s="12"/>
       <c r="B30" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="D30" s="11" t="s">
-        <v>204</v>
-      </c>
-      <c r="F30" s="11"/>
+      <c r="D30" s="13" t="s">
+        <v>214</v>
+      </c>
+      <c r="F30" s="13"/>
       <c r="K30" s="0" t="s">
-        <v>174</v>
+        <v>183</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="10"/>
+      <c r="A31" s="12"/>
       <c r="B31" s="0" t="s">
         <v>86</v>
       </c>
-      <c r="D31" s="11" t="s">
-        <v>205</v>
-      </c>
-      <c r="F31" s="11" t="s">
-        <v>206</v>
+      <c r="D31" s="13" t="s">
+        <v>215</v>
+      </c>
+      <c r="F31" s="13" t="s">
+        <v>216</v>
       </c>
       <c r="K31" s="0" t="s">
-        <v>95</v>
+        <v>186</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="10"/>
+      <c r="A32" s="12"/>
       <c r="B32" s="0" t="s">
         <v>87</v>
       </c>
-      <c r="D32" s="11" t="s">
-        <v>207</v>
-      </c>
-      <c r="F32" s="11"/>
+      <c r="D32" s="13" t="s">
+        <v>217</v>
+      </c>
+      <c r="F32" s="13"/>
       <c r="K32" s="0" t="s">
-        <v>95</v>
+        <v>186</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="10"/>
+      <c r="A33" s="12"/>
       <c r="B33" s="0" t="s">
         <v>88</v>
       </c>
-      <c r="D33" s="11" t="s">
-        <v>208</v>
-      </c>
-      <c r="F33" s="11"/>
+      <c r="D33" s="13" t="s">
+        <v>218</v>
+      </c>
+      <c r="F33" s="13"/>
       <c r="K33" s="0" t="s">
-        <v>95</v>
+        <v>186</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="10"/>
+      <c r="A34" s="12"/>
       <c r="B34" s="0" t="s">
         <v>89</v>
       </c>
-      <c r="D34" s="11" t="s">
-        <v>209</v>
-      </c>
-      <c r="F34" s="11"/>
+      <c r="D34" s="13" t="s">
+        <v>219</v>
+      </c>
+      <c r="F34" s="13"/>
       <c r="K34" s="0" t="s">
-        <v>95</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>
@@ -3423,7 +3788,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.8010204081633"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -3449,22 +3814,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.8010204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>210</v>
+        <v>220</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>211</v>
+        <v>221</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>212</v>
+        <v>222</v>
       </c>
     </row>
   </sheetData>
@@ -3491,121 +3856,121 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.8010204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>213</v>
+        <v>223</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>214</v>
+        <v>224</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>215</v>
+        <v>225</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>216</v>
+        <v>226</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>217</v>
+        <v>166</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>218</v>
+        <v>227</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>219</v>
+        <v>167</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>220</v>
+        <v>123</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>221</v>
+        <v>168</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>222</v>
+        <v>169</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>224</v>
+        <v>171</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>142</v>
+        <v>151</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>

</xml_diff>